<commit_message>
add and update playlists files
genre songs and playlists
</commit_message>
<xml_diff>
--- a/docs/Records and Playlists/playlists.xlsx
+++ b/docs/Records and Playlists/playlists.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
   <si>
     <t>language</t>
   </si>
@@ -116,9 +116,6 @@
     <t>rus_songs_v3</t>
   </si>
   <si>
-    <t>spa_songs_v1</t>
-  </si>
-  <si>
     <t>yid_songs_v1</t>
   </si>
   <si>
@@ -213,13 +210,55 @@
   </si>
   <si>
     <t>eng_songs_v5</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>cla</t>
+  </si>
+  <si>
+    <t>lad</t>
+  </si>
+  <si>
+    <t>pra</t>
+  </si>
+  <si>
+    <t>yiddish</t>
+  </si>
+  <si>
+    <t>mizrahit middle east</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>ladino</t>
+  </si>
+  <si>
+    <t>prayer (piyutim)</t>
+  </si>
+  <si>
+    <t>mizrahit_middle_east_music_v1</t>
+  </si>
+  <si>
+    <t>prayer_songs_v1</t>
+  </si>
+  <si>
+    <t>ladino_songs_v1</t>
+  </si>
+  <si>
+    <t>classical_songs_v1</t>
+  </si>
+  <si>
+    <t>spa_songs_v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,20 +285,6 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF030303"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -372,7 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,13 +425,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -418,11 +436,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -434,7 +452,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -745,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -755,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -766,7 +784,7 @@
     <col min="3" max="3" width="24.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.875" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.25" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
@@ -774,32 +792,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="30" t="s">
-        <v>31</v>
+      <c r="I1" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -815,29 +833,29 @@
       <c r="U1" s="4"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="A2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="19">
+      <c r="H2" s="22"/>
+      <c r="I2" s="16">
         <v>10</v>
       </c>
       <c r="J2" s="6"/>
@@ -854,30 +872,30 @@
       <c r="U2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19">
-        <v>33</v>
+      <c r="B3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16">
+        <v>40</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -893,31 +911,31 @@
       <c r="U3" s="4"/>
     </row>
     <row r="4" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="D4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="16">
         <v>1930</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <v>30</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="16">
         <v>14</v>
       </c>
       <c r="J4" s="6"/>
@@ -934,31 +952,31 @@
       <c r="U4" s="4"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="16">
         <v>1940</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <v>40</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="16">
         <v>12</v>
       </c>
       <c r="J5" s="6"/>
@@ -975,31 +993,31 @@
       <c r="U5" s="4"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="19">
+      <c r="D6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="16">
         <v>1950</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="16">
         <v>50</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="16">
         <v>23</v>
       </c>
       <c r="J6" s="5"/>
@@ -1016,31 +1034,31 @@
       <c r="U6" s="4"/>
     </row>
     <row r="7" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="19">
+      <c r="D7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16">
         <v>1960</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="16">
         <v>60</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="16">
         <v>33</v>
       </c>
       <c r="J7" s="5"/>
@@ -1057,31 +1075,31 @@
       <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="19">
+      <c r="D8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="16">
         <v>1970</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="16">
         <v>70</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <v>21</v>
       </c>
       <c r="J8" s="5"/>
@@ -1098,31 +1116,31 @@
       <c r="U8" s="4"/>
     </row>
     <row r="9" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="19">
+      <c r="D9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="16">
         <v>1930</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="16">
         <v>30</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="16">
         <v>14</v>
       </c>
       <c r="J9" s="5"/>
@@ -1139,31 +1157,31 @@
       <c r="U9" s="4"/>
     </row>
     <row r="10" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="19">
+      <c r="D10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="16">
         <v>1940</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="21" t="s">
+      <c r="F10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="16">
         <v>40</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="16">
         <v>22</v>
       </c>
       <c r="J10" s="5"/>
@@ -1180,31 +1198,31 @@
       <c r="U10" s="4"/>
     </row>
     <row r="11" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="19">
+      <c r="D11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="16">
         <v>1950</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="16">
         <v>50</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="16">
         <v>13</v>
       </c>
       <c r="J11" s="5"/>
@@ -1221,31 +1239,31 @@
       <c r="U11" s="4"/>
     </row>
     <row r="12" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="19">
+      <c r="D12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="16">
         <v>1960</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="F12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="16">
         <v>60</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <v>21</v>
       </c>
       <c r="J12" s="5"/>
@@ -1262,31 +1280,31 @@
       <c r="U12" s="4"/>
     </row>
     <row r="13" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="21" t="s">
+      <c r="B13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="D13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="16">
         <v>1970</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="16">
         <v>70</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="16">
         <v>27</v>
       </c>
       <c r="J13" s="5"/>
@@ -1303,29 +1321,29 @@
       <c r="U13" s="4"/>
     </row>
     <row r="14" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="A14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="E14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16">
         <v>30</v>
       </c>
       <c r="J14" s="5"/>
@@ -1342,29 +1360,29 @@
       <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19">
+      <c r="E15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16">
         <v>46</v>
       </c>
       <c r="J15" s="5"/>
@@ -1381,31 +1399,31 @@
       <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="16">
+        <v>1930</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="19">
-        <v>1930</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="19">
+      <c r="H16" s="16">
         <v>30</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="16">
         <v>12</v>
       </c>
       <c r="J16" s="5"/>
@@ -1422,31 +1440,31 @@
       <c r="U16" s="4"/>
     </row>
     <row r="17" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A17" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="21" t="s">
+      <c r="A17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="16">
+        <v>1940</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="19">
-        <v>1940</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="H17" s="16">
         <v>40</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="16">
         <v>10</v>
       </c>
       <c r="J17" s="5"/>
@@ -1463,31 +1481,31 @@
       <c r="U17" s="4"/>
     </row>
     <row r="18" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A18" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="A18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="16">
+        <v>1950</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="19">
-        <v>1950</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="19">
+      <c r="H18" s="16">
         <v>50</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="16">
         <v>16</v>
       </c>
       <c r="J18" s="5"/>
@@ -1504,31 +1522,31 @@
       <c r="U18" s="4"/>
     </row>
     <row r="19" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A19" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="A19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="16">
+        <v>1960</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="19">
-        <v>1960</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="19">
+      <c r="H19" s="16">
         <v>60</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="16">
         <v>15</v>
       </c>
       <c r="J19" s="5"/>
@@ -1545,31 +1563,31 @@
       <c r="U19" s="4"/>
     </row>
     <row r="20" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A20" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="A20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="16">
+        <v>1970</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="19">
-        <v>1970</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="19">
+      <c r="H20" s="16">
         <v>70</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="16">
         <v>45</v>
       </c>
       <c r="J20" s="5"/>
@@ -1586,31 +1604,31 @@
       <c r="U20" s="4"/>
     </row>
     <row r="21" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="D21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="E21" s="16">
+        <v>1980</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="19">
-        <v>1980</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="19">
+      <c r="H21" s="16">
         <v>80</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="16">
         <v>29</v>
       </c>
       <c r="J21" s="5"/>
@@ -1627,31 +1645,31 @@
       <c r="U21" s="4"/>
     </row>
     <row r="22" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A22" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="31" t="s">
+      <c r="A22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="E22" s="16">
+        <v>1930</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="19">
-        <v>1930</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="19">
+      <c r="H22" s="16">
         <v>30</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="16">
         <v>7</v>
       </c>
       <c r="J22" s="5"/>
@@ -1668,31 +1686,31 @@
       <c r="U22" s="4"/>
     </row>
     <row r="23" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A23" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="31" t="s">
+      <c r="A23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="19">
+      <c r="E23" s="16">
         <v>1940</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="19">
+      <c r="F23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="16">
         <v>40</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="16">
         <v>6</v>
       </c>
       <c r="J23" s="5"/>
@@ -1709,31 +1727,31 @@
       <c r="U23" s="4"/>
     </row>
     <row r="24" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A24" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="31" t="s">
+      <c r="A24" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="19">
+      <c r="E24" s="16">
         <v>1950</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24" s="19">
+      <c r="F24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="16">
         <v>50</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="16">
         <v>14</v>
       </c>
       <c r="J24" s="5"/>
@@ -1750,31 +1768,31 @@
       <c r="U24" s="4"/>
     </row>
     <row r="25" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A25" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="A25" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="19">
+      <c r="E25" s="16">
         <v>1960</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="19" t="s">
+      <c r="F25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="16">
         <v>60</v>
       </c>
-      <c r="H25" s="19">
-        <v>60</v>
-      </c>
-      <c r="I25" s="19">
+      <c r="I25" s="16">
         <v>22</v>
       </c>
       <c r="J25" s="5"/>
@@ -1791,31 +1809,31 @@
       <c r="U25" s="4"/>
     </row>
     <row r="26" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="31" t="s">
+      <c r="D26" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="19">
+      <c r="E26" s="16">
         <v>1970</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="19">
+      <c r="F26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="16">
         <v>70</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="16">
         <v>10</v>
       </c>
       <c r="J26" s="5"/>
@@ -1832,15 +1850,27 @@
       <c r="U26" s="4"/>
     </row>
     <row r="27" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="A27" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16">
+        <v>56</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="6"/>
       <c r="L27" s="10"/>
@@ -1855,15 +1885,27 @@
       <c r="U27" s="4"/>
     </row>
     <row r="28" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="A28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16">
+        <v>22</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="6"/>
       <c r="L28" s="10"/>
@@ -1878,15 +1920,27 @@
       <c r="U28" s="4"/>
     </row>
     <row r="29" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="A29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16">
+        <v>25</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="6"/>
       <c r="L29" s="10"/>
@@ -1901,15 +1955,27 @@
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="A30" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16">
+        <v>26</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1952,7 +2018,7 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="16"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1975,7 +2041,7 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="17"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>

</xml_diff>